<commit_message>
written code to write transient segment data for .sfr file
</commit_message>
<xml_diff>
--- a/MAURICE/test_models/m11_C1_sfr_data.xlsx
+++ b/MAURICE/test_models/m11_C1_sfr_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\hm\MAURICE\test_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A453E312-73DB-4124-9D82-19E40CFC61F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26137CE6-16E0-4E2A-87B2-C6B5AF2CCDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71895" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="5" activeTab="5" xr2:uid="{3815B33F-C467-47DB-BE3E-F164846AD30F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{3815B33F-C467-47DB-BE3E-F164846AD30F}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEM1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
   <si>
     <t>ISEG</t>
   </si>
@@ -632,12 +632,12 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -675,7 +675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-174</v>
       </c>
@@ -726,9 +726,9 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4553</v>
       </c>
@@ -780,7 +780,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4554</v>
       </c>
@@ -806,7 +806,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4677</v>
       </c>
@@ -832,7 +832,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4678</v>
       </c>
@@ -858,7 +858,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4679</v>
       </c>
@@ -884,7 +884,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4680</v>
       </c>
@@ -910,7 +910,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4803</v>
       </c>
@@ -936,7 +936,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4804</v>
       </c>
@@ -962,7 +962,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4805</v>
       </c>
@@ -988,7 +988,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4806</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4929</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4930</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5053</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5054</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5055</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5178</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5179</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5302</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5303</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5304</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5427</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5428</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5551</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5552</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5553</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5554</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5555</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5556</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5557</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5558</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5559</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5682</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5683</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5684</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5807</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5808</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5931</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5932</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5933</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6056</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6057</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6058</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>6181</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6182</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6183</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6184</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6307</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6308</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6309</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6432</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6433</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6434</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6557</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6558</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>6559</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>6560</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6561</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6684</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6685</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6686</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6687</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>6688</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>6811</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>6812</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>6813</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>6814</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>6815</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>6692</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>6693</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>6570</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>6571</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>6448</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>6325</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>6326</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>6203</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>6080</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>6081</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5958</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5959</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>5960</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5837</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5838</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5839</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>5716</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5717</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>5718</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5595</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5596</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5597</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5474</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>5475</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5476</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5477</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5478</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5479</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>5480</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5481</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5359</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5360</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5361</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5362</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>5485</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>5608</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>5609</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>5732</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>5855</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>5978</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>5979</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>6102</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>6103</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>6226</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>6227</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>6228</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>6351</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>6352</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>6353</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>6354</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>6355</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>6478</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>6479</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>6480</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>6481</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>6482</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>6483</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>6484</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>6607</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>6608</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>6609</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>6610</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>6611</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>6612</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>6735</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>6736</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>6737</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>6738</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>6739</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>6740</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>6863</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>6864</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>6865</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>6866</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>6867</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>6868</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>6869</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>6992</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>6993</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>6994</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>6995</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>6996</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>6997</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>6874</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>6875</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>6876</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>6753</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>6754</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>6755</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>6632</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>6633</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>6510</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>6387</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>6388</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>6265</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>6266</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>6143</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>6144</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>6145</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>6268</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>6269</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>6270</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>6271</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>6394</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>6395</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>6518</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>6641</v>
       </c>
@@ -5291,9 +5291,9 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7</v>
       </c>
@@ -5334,9 +5334,9 @@
       <selection activeCell="A2" sqref="A2:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5581,9 +5581,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6424,13 +6424,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F66ED0-3422-4DE9-BF71-3028C78BAFA0}">
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6600,7 +6600,7 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6663,7 +6663,7 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6726,7 +6726,7 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6789,7 +6789,7 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6852,7 +6852,7 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6928,14 +6928,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>19.729999999999997</v>
       </c>
@@ -6953,14 +6953,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>19.729999999999997</v>
       </c>
@@ -6972,15 +6972,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E0C635-67D8-4BB4-AB74-9EF177CF5CDA}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>19.729999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7083,9 +7083,9 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>68</v>
@@ -7122,9 +7122,9 @@
         <v>19.729999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>69</v>
@@ -7154,9 +7154,9 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
@@ -7193,9 +7193,9 @@
         <v>19.729999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>69</v>
@@ -7225,9 +7225,9 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>68</v>
@@ -7264,9 +7264,9 @@
         <v>19.729999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
@@ -7296,9 +7296,9 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>68</v>
@@ -7335,9 +7335,9 @@
         <v>19.729999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>69</v>
@@ -7367,9 +7367,9 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>68</v>
@@ -7406,9 +7406,9 @@
         <v>19.729999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>69</v>
@@ -7437,6 +7437,97 @@
       <c r="J13" s="2">
         <v>3.29</v>
       </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <f>2.21+0.18</f>
+        <v>2.39</v>
+      </c>
+      <c r="E14" s="2">
+        <f>2.21+0.18+1.99</f>
+        <v>4.38</v>
+      </c>
+      <c r="F14" s="2">
+        <f>E14+0.3+0.05</f>
+        <v>4.7299999999999995</v>
+      </c>
+      <c r="G14" s="2">
+        <f>F14+2.57+1.99</f>
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="H14" s="2">
+        <f>G14+3.34+2.63</f>
+        <v>15.259999999999998</v>
+      </c>
+      <c r="I14" s="2">
+        <f>H14+0.1+0.2</f>
+        <v>15.559999999999997</v>
+      </c>
+      <c r="J14" s="2">
+        <f>I14+1.79+0.11+2.27</f>
+        <v>19.729999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3.29</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>